<commit_message>
Add the command WS2812 for a 1st led
</commit_message>
<xml_diff>
--- a/UART_command_list.xlsx
+++ b/UART_command_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Byte 0</t>
   </si>
@@ -145,13 +145,49 @@
   </si>
   <si>
     <t>reg_sel_config_ws2812_led0</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>leds reset_gen</t>
+  </si>
+  <si>
+    <t>en_start led</t>
+  </si>
+  <si>
+    <t>Selection of the led config</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +196,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <strike/>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -483,81 +534,102 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -959,81 +1031,81 @@
   <sheetData>
     <row r="3" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:6" ht="15.75" thickBot="1">
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="2:6" ht="15.75" thickBot="1">
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="10" spans="2:6" ht="15.75" thickBot="1">
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" spans="2:6" ht="15.75" thickBot="1">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1041,16 +1113,16 @@
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -1058,16 +1130,16 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -1086,117 +1158,184 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C5:G33"/>
+  <dimension ref="D2:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" style="1"/>
-    <col min="3" max="3" width="27.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="2" width="11.5703125" style="25"/>
+    <col min="3" max="3" width="27.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="11.5703125" style="25"/>
+    <col min="14" max="14" width="14.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.5703125" style="25"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:5">
-      <c r="D5" s="1" t="s">
+    <row r="2" spans="4:15" ht="16.5" thickBot="1"/>
+    <row r="3" spans="4:15" s="28" customFormat="1" ht="18.75">
+      <c r="D3" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="4:15">
+      <c r="D4" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+    </row>
+    <row r="5" spans="4:15">
+      <c r="D5" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="18:22">
+      <c r="R18" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="S18" s="25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="4:5">
-      <c r="D6" s="1" t="s">
+    <row r="19" spans="18:22">
+      <c r="R19" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="S19" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="4:5">
-      <c r="D7" s="1" t="s">
+    <row r="20" spans="18:22">
+      <c r="R20" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="S20" s="25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="4:5">
-      <c r="D10" s="2" t="s">
+    <row r="23" spans="18:22">
+      <c r="R23" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="S23" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="3:7">
-      <c r="D20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="3:7">
-      <c r="D22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7">
-      <c r="D23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="3:7">
-      <c r="C32" s="1" t="s">
+    <row r="27" spans="18:22">
+      <c r="R27" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="S27" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="T27" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="U27" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="V27" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="4:4">
-      <c r="D33" s="1" t="s">
+    <row r="28" spans="18:22">
+      <c r="S28" s="25" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H4:O4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>